<commit_message>
Aðallega HTML+CSS en líka smávægilegar villur leiðréttar o.s.frv.
</commit_message>
<xml_diff>
--- a/pangea_excel_test.xlsx
+++ b/pangea_excel_test.xlsx
@@ -36,7 +36,7 @@
     <t>Freyja</t>
   </si>
   <si>
-    <t>Mui</t>
+    <t>Muhammed</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Email, gagnagrunnsskorður og alls konar
</commit_message>
<xml_diff>
--- a/pangea_excel_test.xlsx
+++ b/pangea_excel_test.xlsx
@@ -19,34 +19,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Nemandi</t>
   </si>
   <si>
     <t>Kennitala</t>
   </si>
-  <si>
-    <t>Gunnar</t>
-  </si>
-  <si>
-    <t>Sölvi</t>
-  </si>
-  <si>
-    <t>Freyja</t>
-  </si>
-  <si>
-    <t>Muhammed</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +73,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,59 +418,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>9401234498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1320498712</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>123412341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1234</v>
-      </c>
-    </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>